<commit_message>
Code can now limit classroom's times and lecturers' times.
</commit_message>
<xml_diff>
--- a/Main Code/Classroom Occupancy.xlsx
+++ b/Main Code/Classroom Occupancy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/PycharmProjects/AutoTimetable/Main Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F127D5-AF8F-E947-9178-85BE24484249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09A5918-5534-1C42-8A62-32AC3A697009}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{A93ECF93-94E5-4E4A-AECA-6E2408BC5854}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Time</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Classroom G</t>
+  </si>
+  <si>
+    <t>\n</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF2E8855-3F05-C749-97B0-1B7DF6686264}">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -424,7 +427,7 @@
     <col min="8" max="8" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -449,8 +452,11 @@
       <c r="H1">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -475,26 +481,29 @@
       <c r="H2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:H18" ca="1" si="0">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <f t="shared" ref="C3:H3" ca="1" si="0">RANDBETWEEN(0,1)</f>
+        <v>0</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="0"/>
@@ -502,14 +511,17 @@
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -518,31 +530,33 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="C3:H18" ca="1" si="2">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="E4">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="F4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="G4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="H4">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -551,31 +565,34 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="D5">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="F5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="G5">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="H5">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -584,31 +601,34 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="D6">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="E6">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="F6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="G6">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H6">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -617,64 +637,70 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="E7">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="F7">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="G7">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="H7">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="D8">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="E8">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="F8">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="G8">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="H8">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -683,31 +709,34 @@
         <v>0</v>
       </c>
       <c r="C9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="D9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="E9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="F9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="G9">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H9">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -716,64 +745,70 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="D10">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="E10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="F10">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="G10">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H10">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="D11">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="E11">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="F11">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="G11">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="H11">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -782,196 +817,214 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="D12">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="E12">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="F12">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="G12">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="H12">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="D13">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E13">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="F13">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="G13">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="H13">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="D14">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="E14">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="F14">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="G14">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H14">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="D15">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E15">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
       </c>
       <c r="F15">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="G15">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="H15">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="D16">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="E16">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="F16">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="G16">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H16">
-        <f t="shared" ca="1" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="D17">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="E17">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="F17">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="G17">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H17">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -980,31 +1033,34 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>0</v>
       </c>
       <c r="D18">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="E18">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="F18">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="G18">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
       </c>
       <c r="H18">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1014,7 +1070,7 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
@@ -1022,7 +1078,7 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <f t="shared" ca="1" si="1"/>
@@ -1036,18 +1092,21 @@
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
@@ -1063,20 +1122,23 @@
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
@@ -1100,16 +1162,19 @@
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
@@ -1117,7 +1182,7 @@
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
@@ -1125,18 +1190,21 @@
       </c>
       <c r="F22">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1158,7 +1226,7 @@
       </c>
       <c r="F23">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="1"/>
@@ -1166,16 +1234,19 @@
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
@@ -1187,7 +1258,7 @@
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F24">
         <f t="shared" ca="1" si="1"/>
@@ -1201,8 +1272,11 @@
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -1216,11 +1290,11 @@
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25">
         <f t="shared" ca="1" si="1"/>
@@ -1228,20 +1302,23 @@
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
@@ -1249,15 +1326,15 @@
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F26">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G26">
         <f t="shared" ca="1" si="1"/>
@@ -1265,16 +1342,19 @@
       </c>
       <c r="H26">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
@@ -1282,44 +1362,47 @@
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F27">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F28">
         <f t="shared" ca="1" si="1"/>
@@ -1327,14 +1410,17 @@
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -1344,7 +1430,7 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="1"/>
@@ -1356,7 +1442,7 @@
       </c>
       <c r="F29">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="1"/>
@@ -1366,8 +1452,11 @@
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -1385,7 +1474,7 @@
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30">
         <f t="shared" ca="1" si="1"/>
@@ -1399,8 +1488,11 @@
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -1418,22 +1510,25 @@
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -1443,7 +1538,7 @@
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="1"/>
@@ -1451,7 +1546,7 @@
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F32">
         <f t="shared" ca="1" si="1"/>
@@ -1465,8 +1560,11 @@
         <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -1476,7 +1574,7 @@
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="1"/>
@@ -1492,14 +1590,17 @@
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -1509,19 +1610,19 @@
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F34">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="1"/>
@@ -1529,10 +1630,13 @@
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -1542,7 +1646,7 @@
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="1"/>
@@ -1550,7 +1654,7 @@
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F35">
         <f t="shared" ca="1" si="1"/>
@@ -1562,1062 +1666,1161 @@
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
       <c r="B36">
-        <f t="shared" ref="B36:H67" ca="1" si="2">RANDBETWEEN(0,1)</f>
+        <f t="shared" ref="B36:H67" ca="1" si="3">RANDBETWEEN(0,1)</f>
         <v>0</v>
       </c>
       <c r="C36">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="D36">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="E36">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="F36">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="G36">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H36">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="C37">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="D37">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="E37">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="F37">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="G37">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="H37">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C38">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="D38">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E38">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="F38">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="G38">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="H38">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
       <c r="B39">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C39">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D39">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="E39">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="F39">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="G39">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="H39">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
       <c r="B40">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C40">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D40">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="E40">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="F40">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="G40">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H40">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C41">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="D41">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="E41">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="F41">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="G41">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="H41">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="C42">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="D42">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E42">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="F42">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="G42">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="H42">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
       <c r="B43">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="C43">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D43">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="E43">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="F43">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G43">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="H43">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
       <c r="B44">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C44">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="D44">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="E44">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F44">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G44">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="H44">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="C45">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D45">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E45">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="F45">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="G45">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="H45">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="C46">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="D46">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="E46">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="F46">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="G46">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="H46">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="C47">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="D47">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="E47">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="F47">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="G47">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="H47">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="C48">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D48">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="E48">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="F48">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="G48">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="H48">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="C49">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="D49">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="E49">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="F49">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="G49">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="H49">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="C50">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="D50">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="E50">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="F50">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="G50">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="H50">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="C51">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="D51">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="E51">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="F51">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="G51">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="H51">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="C52">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="D52">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="E52">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="F52">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="G52">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="H52">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
       <c r="B53">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="C53">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="D53">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E53">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F53">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G53">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="H53">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
       <c r="B54">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="C54">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D54">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E54">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="F54">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G54">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="H54">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
       <c r="B55">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C55">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D55">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E55">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="F55">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G55">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="H55">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
       <c r="B56">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="C56">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D56">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E56">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="F56">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G56">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="H56">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
       <c r="B57">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="C57">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="D57">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="E57">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="F57">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G57">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="H57">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
       <c r="B58">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C58">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D58">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="E58">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F58">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="G58">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="H58">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
       <c r="B59">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="C59">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="D59">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="E59">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="F59">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="G59">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H59">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>58</v>
       </c>
       <c r="B60">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="C60">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="D60">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E60">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="F60">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G60">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H60">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
       <c r="B61">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="C61">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="D61">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="E61">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="F61">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="G61">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="H61">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
       <c r="B62">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C62">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="D62">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E62">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F62">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="G62">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="H62">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
       <c r="B63">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C63">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="D63">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="E63">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="F63">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="G63">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H63">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62</v>
       </c>
       <c r="B64">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="C64">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="D64">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="E64">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="F64">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="G64">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="H64">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
       <c r="B65">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="C65">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="D65">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="E65">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="F65">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="G65">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="H65">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
       <c r="B66">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
       </c>
       <c r="D66">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="E66">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="F66">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="G66">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H66">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>65</v>
       </c>
       <c r="B67">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C67">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D67">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="E67">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>0</v>
       </c>
       <c r="F67">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G67">
-        <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>0</v>
       </c>
       <c r="H67">
-        <f t="shared" ca="1" si="2"/>
+        <f t="shared" ca="1" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="I67">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Lunchtimes and lecturer time limits implemented.
</commit_message>
<xml_diff>
--- a/Main Code/Classroom Occupancy.xlsx
+++ b/Main Code/Classroom Occupancy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/PycharmProjects/AutoTimetable/Main Code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09A5918-5534-1C42-8A62-32AC3A697009}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08E3EFF-2193-544D-A9E7-CA1054DE1F4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{A93ECF93-94E5-4E4A-AECA-6E2408BC5854}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{A93ECF93-94E5-4E4A-AECA-6E2408BC5854}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -414,7 +414,7 @@
   <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -490,31 +490,24 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <f ca="1">RANDBETWEEN(0,1)</f>
         <v>1</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:H3" ca="1" si="0">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
       <c r="G3">
-        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
       <c r="H3">
-        <f t="shared" ca="1" si="0"/>
         <v>1</v>
       </c>
       <c r="I3">
@@ -526,30 +519,24 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:H35" ca="1" si="1">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="C3:H18" ca="1" si="2">RANDBETWEEN(0,1)</f>
         <v>1</v>
       </c>
       <c r="E4">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="G4">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H4">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="I4">
@@ -561,31 +548,24 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C5">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="D5">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="F5">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="G5">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="I5">
@@ -597,32 +577,25 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="D6">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="F6">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H6">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -633,32 +606,25 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="E7">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="F7">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="G7">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -669,32 +635,25 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C8">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="E8">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="F8">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="G8">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H8">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -705,32 +664,25 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="E9">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="F9">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="G9">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H9">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -741,31 +693,24 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C10">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="E10">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G10">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H10">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="I10">
@@ -777,31 +722,24 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="D11">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="E11">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="G11">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="I11">
@@ -813,32 +751,25 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C12">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -849,31 +780,24 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C13">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="D13">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="F13">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="G13">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="I13">
@@ -885,32 +809,25 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C14">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="D14">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="E14">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="G14">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H14">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -921,32 +838,25 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C15">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="D15">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="G15">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H15">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -957,32 +867,25 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="F16">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H16">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -993,31 +896,24 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C17">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="D17">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="E17">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="F17">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="G17">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H17">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="I17">
@@ -1029,32 +925,25 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C18">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="E18">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="F18">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="G18">
-        <f t="shared" ca="1" si="2"/>
         <v>1</v>
       </c>
       <c r="H18">
-        <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1065,31 +954,24 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="D19">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="E19">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="F19">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="H19">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="I19">
@@ -1101,32 +983,25 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="F20">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="G20">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1137,31 +1012,24 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="E21">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="G21">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="H21">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="I21">
@@ -1173,31 +1041,24 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C22">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G22">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="I22">
@@ -1209,31 +1070,24 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="F23">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="I23">
@@ -1245,31 +1099,24 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="D24">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="G24">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="H24">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="I24">
@@ -1281,31 +1128,24 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="D25">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="F25">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="H25">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="I25">
@@ -1317,32 +1157,25 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C26">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="D26">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F26">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="G26">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -1353,32 +1186,25 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C27">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="D27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F27">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="G27">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="H27">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -1389,32 +1215,25 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C28">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="G28">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -1425,32 +1244,25 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="H29">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -1461,31 +1273,24 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C30">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="D30">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="E30">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="F30">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="G30">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="I30">
@@ -1497,32 +1302,25 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C31">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="D31">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="E31">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="F31">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="H31">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -1533,32 +1331,25 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C32">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="D32">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F32">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H32">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32">
         <v>0</v>
@@ -1569,31 +1360,24 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="F33">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="G33">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="H33">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="I33">
@@ -1605,32 +1389,25 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C34">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="F34">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G34">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="H34">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -1641,32 +1418,25 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="C35">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="D35">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="F35">
-        <f t="shared" ca="1" si="1"/>
         <v>1</v>
       </c>
       <c r="G35">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35">
         <v>0</v>
@@ -1677,32 +1447,25 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <f t="shared" ref="B36:H67" ca="1" si="3">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C36">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F36">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G36">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H36">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -1713,32 +1476,25 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C37">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F37">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G37">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
         <v>0</v>
@@ -1749,31 +1505,24 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C38">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E38">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F38">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H38">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I38">
@@ -1785,32 +1534,25 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C39">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D39">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E39">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F39">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I39">
         <v>0</v>
@@ -1821,32 +1563,25 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C40">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D40">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F40">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G40">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H40">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I40">
         <v>0</v>
@@ -1857,32 +1592,25 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C41">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F41">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G41">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -1893,31 +1621,24 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C42">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E42">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G42">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I42">
@@ -1929,32 +1650,25 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C43">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D43">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F43">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G43">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H43">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -1965,31 +1679,24 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C44">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D44">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E44">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F44">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G44">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H44">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I44">
@@ -2001,31 +1708,24 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C45">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D45">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E45">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F45">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G45">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I45">
@@ -2037,31 +1737,24 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C46">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D46">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F46">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G46">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H46">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I46">
@@ -2073,31 +1766,24 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C47">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F47">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G47">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H47">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I47">
@@ -2109,32 +1795,25 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C48">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D48">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F48">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G48">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H48">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I48">
         <v>0</v>
@@ -2145,31 +1824,24 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C49">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F49">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G49">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H49">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I49">
@@ -2181,31 +1853,24 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C50">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F50">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G50">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H50">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I50">
@@ -2217,31 +1882,24 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E51">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F51">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G51">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H51">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I51">
@@ -2253,32 +1911,25 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C52">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D52">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E52">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F52">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G52">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H52">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I52">
         <v>0</v>
@@ -2289,31 +1940,24 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C53">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E53">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F53">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G53">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H53">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I53">
@@ -2325,31 +1969,24 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C54">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D54">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E54">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F54">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G54">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H54">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I54">
@@ -2361,31 +1998,24 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C55">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D55">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E55">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F55">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G55">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I55">
@@ -2397,31 +2027,24 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C56">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D56">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E56">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F56">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G56">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H56">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I56">
@@ -2433,32 +2056,25 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C57">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E57">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F57">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G57">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I57">
         <v>0</v>
@@ -2469,31 +2085,24 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C58">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D58">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F58">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G58">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H58">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I58">
@@ -2505,31 +2114,24 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C59">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E59">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F59">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G59">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H59">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I59">
@@ -2541,31 +2143,24 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C60">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E60">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F60">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G60">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H60">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I60">
@@ -2577,32 +2172,25 @@
         <v>59</v>
       </c>
       <c r="B61">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C61">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D61">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E61">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F61">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G61">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I61">
         <v>0</v>
@@ -2613,32 +2201,25 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C62">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D62">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E62">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F62">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G62">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H62">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I62">
         <v>0</v>
@@ -2649,31 +2230,24 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C63">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D63">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F63">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G63">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H63">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I63">
@@ -2685,32 +2259,25 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C64">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D64">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="F64">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G64">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H64">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I64">
         <v>0</v>
@@ -2721,32 +2288,25 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C65">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D65">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="E65">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F65">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G65">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H65">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I65">
         <v>0</v>
@@ -2757,32 +2317,25 @@
         <v>64</v>
       </c>
       <c r="B66">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C66">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D66">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F66">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G66">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="H66">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I66">
         <v>0</v>
@@ -2793,31 +2346,24 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="C67">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="D67">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E67">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F67">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="G67">
-        <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67">
-        <f t="shared" ca="1" si="3"/>
         <v>1</v>
       </c>
       <c r="I67">

</xml_diff>